<commit_message>
Update ieee39_uc load scale
</commit_message>
<xml_diff>
--- a/ams/cases/ieee39/ieee39_uc.xlsx
+++ b/ams/cases/ieee39/ieee39_uc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/ams/ams/cases/ieee39/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA2BEA4-800F-9446-8912-DDC06445EBBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2FA6D43-D2FA-5441-91D8-969456D1FCE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21600" yWindow="7420" windowWidth="21600" windowHeight="18940" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21600" yWindow="6320" windowWidth="21600" windowHeight="18940" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="14" r:id="rId1"/>
@@ -29,12 +29,25 @@
     <sheet name="SR" sheetId="16" r:id="rId14"/>
     <sheet name="NSR" sheetId="17" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="415">
   <si>
     <t>idx</t>
   </si>
@@ -786,9 +799,6 @@
     <t>GCost_10</t>
   </si>
   <si>
-    <t>GCost_0</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -1125,33 +1135,6 @@
     <t>PV_39</t>
   </si>
   <si>
-    <t>1, 1, 1</t>
-  </si>
-  <si>
-    <t>1.005, 1.005, 1.005</t>
-  </si>
-  <si>
-    <t>1.01, 1.01, 1.01</t>
-  </si>
-  <si>
-    <t>1.015, 1.015, 1.015</t>
-  </si>
-  <si>
-    <t>1.02, 1.02, 1.02</t>
-  </si>
-  <si>
-    <t>1.025, 1.025, 1.025</t>
-  </si>
-  <si>
-    <t>1.03, 1.03, 1.03</t>
-  </si>
-  <si>
-    <t>1.035, 1.035, 1.035</t>
-  </si>
-  <si>
-    <t>1.04, 1.04, 1.04</t>
-  </si>
-  <si>
     <t>demand</t>
   </si>
   <si>
@@ -1171,6 +1154,144 @@
   </si>
   <si>
     <t>NSR3</t>
+  </si>
+  <si>
+    <t>0.948, 0.948, 0.948</t>
+  </si>
+  <si>
+    <t>0.934, 0.934, 0.934</t>
+  </si>
+  <si>
+    <t>0.918, 0.918, 0.918</t>
+  </si>
+  <si>
+    <t>0.924, 0.924, 0.924</t>
+  </si>
+  <si>
+    <t>0.927, 0.927, 0.927</t>
+  </si>
+  <si>
+    <t>0.976, 0.976, 0.976</t>
+  </si>
+  <si>
+    <t>1.043, 1.043, 1.043</t>
+  </si>
+  <si>
+    <t>1.064, 1.064, 1.064</t>
+  </si>
+  <si>
+    <t>1.072, 1.072, 1.072</t>
+  </si>
+  <si>
+    <t>1.097, 1.097, 1.097</t>
+  </si>
+  <si>
+    <t>1.133, 1.133, 1.133</t>
+  </si>
+  <si>
+    <t>1.137, 1.137, 1.137</t>
+  </si>
+  <si>
+    <t>1.175, 1.175, 1.175</t>
+  </si>
+  <si>
+    <t>1.216, 1.216, 1.216</t>
+  </si>
+  <si>
+    <t>1.268, 1.268, 1.268</t>
+  </si>
+  <si>
+    <t>1.338, 1.338, 1.338</t>
+  </si>
+  <si>
+    <t>1.409, 1.409, 1.409</t>
+  </si>
+  <si>
+    <t>1.429, 1.429, 1.429</t>
+  </si>
+  <si>
+    <t>1.400, 1.400, 1.400</t>
+  </si>
+  <si>
+    <t>1.363, 1.363, 1.363</t>
+  </si>
+  <si>
+    <t>1.306, 1.306, 1.306</t>
+  </si>
+  <si>
+    <t>1.195, 1.195, 1.195</t>
+  </si>
+  <si>
+    <t>1.108, 1.108, 1.108</t>
+  </si>
+  <si>
+    <t>1.000, 1.000, 1.000</t>
+  </si>
+  <si>
+    <t>0.989, 0.989, 0.989</t>
+  </si>
+  <si>
+    <t>0.972, 0.972, 0.972</t>
+  </si>
+  <si>
+    <t>0.959, 0.959, 0.959</t>
+  </si>
+  <si>
+    <t>0.967, 0.967, 0.967</t>
+  </si>
+  <si>
+    <t>1.038, 1.038, 1.038</t>
+  </si>
+  <si>
+    <t>1.112, 1.112, 1.112</t>
+  </si>
+  <si>
+    <t>1.135, 1.135, 1.135</t>
+  </si>
+  <si>
+    <t>1.163, 1.163, 1.163</t>
+  </si>
+  <si>
+    <t>1.210, 1.210, 1.210</t>
+  </si>
+  <si>
+    <t>1.261, 1.261, 1.261</t>
+  </si>
+  <si>
+    <t>1.303, 1.303, 1.303</t>
+  </si>
+  <si>
+    <t>1.341, 1.341, 1.341</t>
+  </si>
+  <si>
+    <t>1.371, 1.371, 1.371</t>
+  </si>
+  <si>
+    <t>1.438, 1.438, 1.438</t>
+  </si>
+  <si>
+    <t>1.489, 1.489, 1.489</t>
+  </si>
+  <si>
+    <t>1.553, 1.553, 1.553</t>
+  </si>
+  <si>
+    <t>1.560, 1.560, 1.560</t>
+  </si>
+  <si>
+    <t>1.538, 1.538, 1.538</t>
+  </si>
+  <si>
+    <t>1.481, 1.481, 1.481</t>
+  </si>
+  <si>
+    <t>1.406, 1.406, 1.406</t>
+  </si>
+  <si>
+    <t>1.284, 1.284, 1.284</t>
+  </si>
+  <si>
+    <t>1.150, 1.150, 1.150</t>
   </si>
 </sst>
 </file>
@@ -1604,16 +1725,16 @@
         <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>349</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1621,10 +1742,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>351</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>352</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -1655,180 +1776,180 @@
         <v>233</v>
       </c>
       <c r="D1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E1" t="s">
         <v>273</v>
-      </c>
-      <c r="E1" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C7" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C8" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C9" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C10" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C11" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -1841,9 +1962,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="185" workbookViewId="0">
+    <sheetView zoomScale="185" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K14" sqref="K14"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1894,10 +2015,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="E2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -1929,10 +2050,10 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -1964,10 +2085,10 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -1999,10 +2120,10 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -2034,10 +2155,10 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -2069,10 +2190,10 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F7">
         <v>2</v>
@@ -2104,10 +2225,10 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E8" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F8">
         <v>2</v>
@@ -2139,10 +2260,10 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F9">
         <v>2</v>
@@ -2174,10 +2295,10 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -2209,10 +2330,10 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E11" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F11">
         <v>2</v>
@@ -2236,6 +2357,7 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2244,7 +2366,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView zoomScale="159" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2263,343 +2385,343 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>363</v>
+        <v>392</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>368</v>
+        <v>379</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>367</v>
+        <v>380</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>366</v>
+        <v>381</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>365</v>
+        <v>382</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>366</v>
+        <v>383</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>367</v>
+        <v>384</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>368</v>
+        <v>385</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>369</v>
+        <v>386</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>370</v>
+        <v>387</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>371</v>
+        <v>388</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>370</v>
+        <v>389</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>369</v>
+        <v>390</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>368</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -2612,8 +2734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D48AD92-083E-E846-8F62-C9A43521848F}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2632,343 +2754,343 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>363</v>
+        <v>392</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>364</v>
+        <v>393</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>365</v>
+        <v>394</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>366</v>
+        <v>395</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>367</v>
+        <v>396</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>368</v>
+        <v>396</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>369</v>
+        <v>397</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>370</v>
+        <v>398</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>371</v>
+        <v>399</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>370</v>
+        <v>400</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>369</v>
+        <v>401</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>302</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>304</v>
-      </c>
       <c r="C13" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>368</v>
+        <v>402</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>304</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>306</v>
-      </c>
       <c r="C14" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>367</v>
+        <v>403</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>306</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>308</v>
-      </c>
       <c r="C15" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>366</v>
+        <v>404</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>308</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>310</v>
-      </c>
       <c r="C16" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>365</v>
+        <v>405</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>310</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>312</v>
-      </c>
       <c r="C17" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>366</v>
+        <v>406</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>312</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>314</v>
-      </c>
       <c r="C18" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>367</v>
+        <v>407</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>314</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>316</v>
-      </c>
       <c r="C19" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>368</v>
+        <v>408</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>316</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>318</v>
-      </c>
       <c r="C20" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>369</v>
+        <v>409</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>318</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>320</v>
-      </c>
       <c r="C21" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>370</v>
+        <v>410</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>320</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>322</v>
-      </c>
       <c r="C22" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>371</v>
+        <v>411</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>322</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>324</v>
-      </c>
       <c r="C23" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>370</v>
+        <v>412</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>324</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>326</v>
-      </c>
       <c r="C24" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>369</v>
+        <v>413</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>326</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>328</v>
-      </c>
       <c r="C25" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>368</v>
+        <v>414</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -3006,7 +3128,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>11</v>
@@ -3017,19 +3139,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="C2" s="8">
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="E2" s="8">
         <v>0.03</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -3037,19 +3159,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="C3" s="8">
         <v>1</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="E3" s="8">
         <v>0.03</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -3057,19 +3179,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="C4" s="8">
         <v>1</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="E4" s="8">
         <v>0.03</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -3101,7 +3223,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>11</v>
@@ -3112,19 +3234,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="C2" s="8">
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="E2" s="8">
         <v>0.05</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -3132,19 +3254,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="C3" s="8">
         <v>1</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="E3" s="8">
         <v>0.05</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -3152,23 +3274,24 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="C4" s="8">
         <v>1</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="E4" s="8">
         <v>0.05</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3265,7 +3388,7 @@
         <v>2</v>
       </c>
       <c r="M2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -3306,7 +3429,7 @@
         <v>2</v>
       </c>
       <c r="M3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -3347,7 +3470,7 @@
         <v>2</v>
       </c>
       <c r="M4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -3388,7 +3511,7 @@
         <v>1</v>
       </c>
       <c r="M5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -3429,7 +3552,7 @@
         <v>1</v>
       </c>
       <c r="M6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -3470,7 +3593,7 @@
         <v>1</v>
       </c>
       <c r="M7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -3511,7 +3634,7 @@
         <v>1</v>
       </c>
       <c r="M8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -3552,7 +3675,7 @@
         <v>1</v>
       </c>
       <c r="M9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -3593,7 +3716,7 @@
         <v>1</v>
       </c>
       <c r="M10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -3634,7 +3757,7 @@
         <v>1</v>
       </c>
       <c r="M11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -3675,7 +3798,7 @@
         <v>1</v>
       </c>
       <c r="M12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -3716,7 +3839,7 @@
         <v>1</v>
       </c>
       <c r="M13" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -3757,7 +3880,7 @@
         <v>1</v>
       </c>
       <c r="M14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -3798,7 +3921,7 @@
         <v>1</v>
       </c>
       <c r="M15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -3839,7 +3962,7 @@
         <v>3</v>
       </c>
       <c r="M16" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -3880,7 +4003,7 @@
         <v>3</v>
       </c>
       <c r="M17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -3921,7 +4044,7 @@
         <v>2</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -3962,7 +4085,7 @@
         <v>2</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -4003,7 +4126,7 @@
         <v>3</v>
       </c>
       <c r="M20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -4044,7 +4167,7 @@
         <v>3</v>
       </c>
       <c r="M21" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -4085,7 +4208,7 @@
         <v>3</v>
       </c>
       <c r="M22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -4126,7 +4249,7 @@
         <v>3</v>
       </c>
       <c r="M23" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
@@ -4167,7 +4290,7 @@
         <v>3</v>
       </c>
       <c r="M24" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -4208,7 +4331,7 @@
         <v>3</v>
       </c>
       <c r="M25" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -4249,7 +4372,7 @@
         <v>2</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
@@ -4290,7 +4413,7 @@
         <v>2</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -4331,7 +4454,7 @@
         <v>2</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
@@ -4372,7 +4495,7 @@
         <v>3</v>
       </c>
       <c r="M29" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
@@ -4413,7 +4536,7 @@
         <v>3</v>
       </c>
       <c r="M30" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
@@ -4454,7 +4577,7 @@
         <v>2</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
@@ -4495,7 +4618,7 @@
         <v>1</v>
       </c>
       <c r="M32" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
@@ -4536,7 +4659,7 @@
         <v>1</v>
       </c>
       <c r="M33" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -4577,7 +4700,7 @@
         <v>3</v>
       </c>
       <c r="M34" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
@@ -4618,7 +4741,7 @@
         <v>3</v>
       </c>
       <c r="M35" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
@@ -4659,7 +4782,7 @@
         <v>3</v>
       </c>
       <c r="M36" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
@@ -4700,7 +4823,7 @@
         <v>3</v>
       </c>
       <c r="M37" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
@@ -4741,7 +4864,7 @@
         <v>2</v>
       </c>
       <c r="M38" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
@@ -4782,7 +4905,7 @@
         <v>3</v>
       </c>
       <c r="M39" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
@@ -4823,7 +4946,7 @@
         <v>1</v>
       </c>
       <c r="M40" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -5674,13 +5797,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E2">
         <v>1500</v>
@@ -5895,13 +6018,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E2">
         <v>1040</v>
@@ -5996,13 +6119,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E3">
         <v>725</v>
@@ -6097,13 +6220,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E4">
         <v>652</v>
@@ -6198,13 +6321,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E5">
         <v>508</v>
@@ -6299,13 +6422,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E6">
         <v>687</v>
@@ -6400,13 +6523,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E7">
         <v>580</v>
@@ -6501,13 +6624,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E8">
         <v>564</v>
@@ -6602,13 +6725,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E9">
         <v>865</v>
@@ -6703,13 +6826,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E10">
         <v>1100</v>
@@ -10616,30 +10739,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>261</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>252</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -10650,10 +10773,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -10687,16 +10810,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -10704,13 +10827,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -10718,13 +10841,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -10756,10 +10879,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>268</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>269</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>11</v>
@@ -10767,16 +10890,16 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E2" s="2">
         <v>0.05</v>
@@ -10785,7 +10908,7 @@
         <v>0.05</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -10793,13 +10916,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E3" s="2">
         <v>0.05</v>
@@ -10808,7 +10931,7 @@
         <v>0.05</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -10816,13 +10939,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E4" s="2">
         <v>0.05</v>
@@ -10831,7 +10954,7 @@
         <v>0.05</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>